<commit_message>
upload functions for paradiso, part 1
</commit_message>
<xml_diff>
--- a/knowledge_representation/grasp analysis.xlsx
+++ b/knowledge_representation/grasp analysis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mytomorrows/Documents/VU/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mytomorrows/Documents/VU/pepper/knowledge_representation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFE2888-E5EF-C545-9887-E3370ABB580F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4620903-1983-2742-A5BF-B5F7F377A36F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="68">
   <si>
     <t>subject</t>
   </si>
@@ -141,12 +141,6 @@
     <t>sem</t>
   </si>
   <si>
-    <t>Entity</t>
-  </si>
-  <si>
-    <t>prov</t>
-  </si>
-  <si>
     <t>NOTE</t>
   </si>
   <si>
@@ -229,6 +223,12 @@
   </si>
   <si>
     <t>links any entity to an agent -&gt; mention must be an entity</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>has time and has actor and has subevent</t>
   </si>
 </sst>
 </file>
@@ -281,13 +281,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,7 +606,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,7 +653,7 @@
         <v>21</v>
       </c>
       <c r="K1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L1" t="s">
         <v>3</v>
@@ -673,7 +673,7 @@
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -685,20 +685,20 @@
         <v>23</v>
       </c>
       <c r="K3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E4" t="s">
@@ -714,16 +714,16 @@
         <v>36</v>
       </c>
       <c r="K4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E5" t="s">
@@ -739,7 +739,7 @@
         <v>23</v>
       </c>
       <c r="K5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -762,10 +762,10 @@
         <v>23</v>
       </c>
       <c r="K6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -788,7 +788,7 @@
         <v>20</v>
       </c>
       <c r="K7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -811,39 +811,39 @@
         <v>20</v>
       </c>
       <c r="K8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D9" s="1"/>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I10" t="s">
         <v>8</v>
@@ -852,15 +852,18 @@
         <v>36</v>
       </c>
       <c r="K10" t="s">
-        <v>58</v>
+        <v>54</v>
+      </c>
+      <c r="L10" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="2" t="s">
         <v>20</v>
       </c>
@@ -877,7 +880,7 @@
         <v>36</v>
       </c>
       <c r="K11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -892,20 +895,20 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="B13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -916,7 +919,7 @@
         <v>31</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>20</v>
@@ -949,13 +952,13 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -969,10 +972,10 @@
         <v>4</v>
       </c>
       <c r="H18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -986,7 +989,7 @@
         <v>5</v>
       </c>
       <c r="H19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1000,7 +1003,7 @@
         <v>10</v>
       </c>
       <c r="H20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1025,15 +1028,15 @@
         <v>24</v>
       </c>
       <c r="G22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -1044,7 +1047,7 @@
         <v>4</v>
       </c>
       <c r="H24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -1061,10 +1064,10 @@
         <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -1072,19 +1075,19 @@
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D26" t="s">
         <v>22</v>
       </c>
       <c r="E26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
align ontology and triple extraction/query
</commit_message>
<xml_diff>
--- a/knowledge_representation/grasp analysis.xlsx
+++ b/knowledge_representation/grasp analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mytomorrows/Documents/VU/pepper/knowledge_representation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4620903-1983-2742-A5BF-B5F7F377A36F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6660F673-1621-7C47-BEF1-C41711BFCA16}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="63">
   <si>
     <t>subject</t>
   </si>
@@ -51,9 +51,6 @@
     <t>grasp</t>
   </si>
   <si>
-    <t>grasp?</t>
-  </si>
-  <si>
     <t>chat</t>
   </si>
   <si>
@@ -144,12 +141,6 @@
     <t>NOTE</t>
   </si>
   <si>
-    <t>remove source</t>
-  </si>
-  <si>
-    <t>no grasp actor, only sem actor</t>
-  </si>
-  <si>
     <t>prov:wasAttributedTo</t>
   </si>
   <si>
@@ -162,9 +153,6 @@
     <t>Add isRelativeOf agent and agent</t>
   </si>
   <si>
-    <t>remove grasp</t>
-  </si>
-  <si>
     <t>Map 'leolani' to robot (self)</t>
   </si>
   <si>
@@ -204,12 +192,6 @@
     <t>can be defined by inference</t>
   </si>
   <si>
-    <t>done</t>
-  </si>
-  <si>
-    <t>questions still</t>
-  </si>
-  <si>
     <t>define statement, is attribution for (inverse of has attribution)</t>
   </si>
   <si>
@@ -229,6 +211,9 @@
   </si>
   <si>
     <t>has time and has actor and has subevent</t>
+  </si>
+  <si>
+    <t>has time and has actor</t>
   </si>
 </sst>
 </file>
@@ -602,11 +587,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -635,25 +620,25 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
       <c r="J1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="L1" t="s">
         <v>3</v>
@@ -664,16 +649,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -682,10 +667,10 @@
         <v>6</v>
       </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -693,41 +678,41 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
         <v>7</v>
       </c>
       <c r="J4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
@@ -736,10 +721,10 @@
         <v>6</v>
       </c>
       <c r="J5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -747,25 +732,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="L6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -773,22 +758,22 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I7" t="s">
         <v>7</v>
       </c>
       <c r="J7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -796,406 +781,425 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I8" t="s">
         <v>7</v>
       </c>
       <c r="J8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D9" s="1"/>
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
       <c r="G9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="D10" s="1"/>
+      <c r="H10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" t="s">
+        <v>50</v>
+      </c>
+      <c r="L10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
         <v>17</v>
       </c>
-      <c r="H10" t="s">
-        <v>49</v>
-      </c>
-      <c r="I10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" t="s">
-        <v>36</v>
-      </c>
-      <c r="K10" t="s">
-        <v>54</v>
-      </c>
-      <c r="L10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" t="s">
-        <v>8</v>
-      </c>
-      <c r="J11" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" t="s">
-        <v>65</v>
-      </c>
-    </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>20</v>
+      <c r="A14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G17" t="s">
-        <v>38</v>
-      </c>
-      <c r="H17" t="s">
-        <v>39</v>
-      </c>
-      <c r="L17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" t="s">
-        <v>40</v>
-      </c>
-      <c r="L18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="H19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" t="s">
-        <v>42</v>
-      </c>
-      <c r="H22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="H24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" t="s">
-        <v>58</v>
-      </c>
-      <c r="H25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" t="s">
-        <v>64</v>
-      </c>
-      <c r="H26" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" t="s">
-        <v>29</v>
+      <c r="C32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" t="s">
         <v>28</v>
-      </c>
-      <c r="C34" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
         <v>28</v>
       </c>
-      <c r="C35" t="s">
-        <v>24</v>
-      </c>
-      <c r="E35" t="s">
-        <v>29</v>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C11:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
more adjustments to KR
</commit_message>
<xml_diff>
--- a/knowledge_representation/grasp analysis.xlsx
+++ b/knowledge_representation/grasp analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mytomorrows/Documents/VU/pepper/knowledge_representation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6660F673-1621-7C47-BEF1-C41711BFCA16}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D760AD-E093-A647-B818-083894693106}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -591,7 +591,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomLeft" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -825,7 +825,7 @@
         <v>45</v>
       </c>
       <c r="I10" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="J10" t="s">
         <v>35</v>
@@ -857,7 +857,7 @@
         <v>8</v>
       </c>
       <c r="I11" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="J11" t="s">
         <v>35</v>

</xml_diff>